<commit_message>
Table of index/paramter formulas for verification
</commit_message>
<xml_diff>
--- a/vignettes/stability.xlsx
+++ b/vignettes/stability.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="51">
   <si>
     <t>function</t>
   </si>
@@ -30,10 +30,6 @@
   </si>
   <si>
     <t>xxxx</t>
-  </si>
-  <si>
-    <t>Sums of the
-absolute value of the IPC scores ($SIPC$)</t>
   </si>
   <si>
     <t>[@sneller_repeatability_1997]</t>
@@ -43,12 +39,6 @@
 Where, $Y_{ij}$ is the yield of $i$^th^ genotype in $j$^th^ environment, $\mu$ is the grand mean, $\alpha_{i}$ is the genotype deviation from the grand mean, $\beta_{j}$ is the environment deviation, $N$ is the number of significant IPCAs (number of IPC that were retained in the AMMI model via F tests), $\lambda_{n}$ is the is the singular value for interaction principal component (IPC) $n$ and correspondingly $\lambda_{n}^{2}$  is its eigen value, $\gamma_{in}$ is the eigenvector value for $i$^th^ genotype, $\delta_{jn}$  is the eigenvector value for $j$^th^ environment and $\rho_{ij}$ is the residual.</t>
   </si>
   <si>
-    <t>$$EV = \sum_{n=1}^{N}\frac{\gamma_{in}^2}{N}$$</t>
-  </si>
-  <si>
-    <t>$EV$ stability parameter</t>
-  </si>
-  <si>
     <t>AMMI equation</t>
   </si>
   <si>
@@ -61,9 +51,6 @@
     <t>[@zobel_stress_1994]</t>
   </si>
   <si>
-    <t>$AMGE$ stability parameter</t>
-  </si>
-  <si>
     <t>AMGE.AMMI</t>
   </si>
   <si>
@@ -73,22 +60,162 @@
     <t>Sneller</t>
   </si>
   <si>
-    <t>$$SIPC = \sum_{n=1}^{N} \left | \lambda_{n}^{0.5}\gamma_{in} \right |$$
-$$SIPC = \sum_{n=1}^{N}\left | IPCA_{n}} \right |$$</t>
-  </si>
-  <si>
-    <t>$$AMGE = \sum_{n=1}^{N}\sum_{i=1}^{G}\lambda_{n}\gamma_{in}\delta_{jn}$$
-Where, {M} is the number of environments</t>
-  </si>
-  <si>
-    <t>AWAI ??</t>
+    <t>AMMI stability value (ASV)</t>
+  </si>
+  <si>
+    <t>Modified AMMI stability value (ASV)</t>
+  </si>
+  <si>
+    <t>[@zali_evaluation_2012]</t>
+  </si>
+  <si>
+    <t>[@annicchiarico_joint_1997]</t>
+  </si>
+  <si>
+    <t>[@zhang_analysis_1998]</t>
+  </si>
+  <si>
+    <t>agricolae::index.AMMI</t>
+  </si>
+  <si>
+    <t>MASV.AMMI</t>
+  </si>
+  <si>
+    <t>$$MASV = \sqrt{\sum_{n=1}^{N'-1}\left (\frac{SSIPC_{n}}{SSIPC_{n+1}} \times PC_{n}  \right )^2   + \left (PC_{N'}  \right )^2} $$</t>
+  </si>
+  <si>
+    <t>$$Za = \sum_{i=1}^{N'}\left | \theta_{n}\gamma_{in} \right |$$</t>
+  </si>
+  <si>
+    <t>The unsquared Euclidean distance from the origin of significant IPC axes (D) in the AMMI model.
+$$D_{a} = \sqrt{\sum_{n=1}^{N'}(\lambda_{n}\gamma_{in})^2}$$</t>
+  </si>
+  <si>
+    <t>Distance from the coordinate point to the origin in a two dimensional scattergram generated by plotting of IPC1 score against IPC2 score.
+$$ASV = \sqrt{\left (\frac{SSIPC_{1}}{SSIPC_{2}}\times PC_{1}  \right )^2   + \left (PC_{2}  \right )^2} $$</t>
+  </si>
+  <si>
+    <t>Stability measure based on fitted AMMI model $FA$</t>
+  </si>
+  <si>
+    <t>$$FA = \sum_{n=1}^{N'}\lambda_{n}^{2}\gamma_{in}^{2}$$</t>
+  </si>
+  <si>
+    <t>$FP$</t>
+  </si>
+  <si>
+    <t>[@raju_study_2002; @zali_evaluation_2012]</t>
+  </si>
+  <si>
+    <t>[@wricke_method_1962; @raju_study_2002; @zali_evaluation_2012]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$D_{a}$ </t>
+  </si>
+  <si>
+    <t>$B$</t>
+  </si>
+  <si>
+    <t>Equivalent to $FA$, when the first two IPC axes are considered for computation.
+$$B = \sum_{n=1}^{2}\lambda_{n}^{2}\gamma_{in}^{2}$$
+Stability comparisons based on this measure will be equivalent to the comparisons based on biplot with first two IPC axes.</t>
+  </si>
+  <si>
+    <t>Equivalent to $FA$, when all the IPC axes in the AMMI model are considered for computation.
+$$W_{AMMI} = \sum_{n=1}^{N}\lambda_{n}^{2}\gamma_{in}^{2}$$
+Equivalent to Wricke's ecovalence.</t>
+  </si>
+  <si>
+    <t>$$AMGE = \sum_{j=1}^{E} \sum_{n=1}^{N'} \lambda_{n} \gamma_{in} \delta_{jn}$$</t>
+  </si>
+  <si>
+    <t>$$AV_{AMGE} = \sum_{j=1}^{E} \sum_{n=1}^{N'} \left |\lambda_{n} \gamma_{in} \delta_{jn}  \right |$$</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Equivalent to $FA$, when only the first IPC axis is considered for computation. 
+$$FP = \lambda_{1}^{2}\gamma_{i1}^{2}$$
+As  $\lambda_{1}^{2}$ will be same for all the genotypes, the absolute value of $gamma_{i1}$ alone is sufficient for comparison. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> So this is also equivalent to the comparison based on biplot with first IPC axis.</t>
+    </r>
+  </si>
+  <si>
+    <t>Sums of the absolute value of the IPC scores ($SIPC$)</t>
+  </si>
+  <si>
+    <t>$$SIPC = \sum_{n=1}^{N'} \left | \lambda_{n}^{0.5}\gamma_{in} \right |$$
+$$SIPC = \sum_{n=1}^{N'}\left | IPC_{n} \right |$$</t>
+  </si>
+  <si>
+    <t>The distance of IPC  point  with  origin  in space. (AMMI stability index)
+$$D_{z} = \sqrt{\sum_{n=1}^{N'}\gamma_{in}^{2}}$$</t>
+  </si>
+  <si>
+    <t>[@purchase_parametric_1997; @purchase_use_1999; @purchase_genotype_2000]</t>
+  </si>
+  <si>
+    <t>AMMI Stability Index ($ASI$)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">AMMI statistic coefficient or AMMI distance or AMMI stability index </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">$D_{z}$ </t>
+    </r>
+  </si>
+  <si>
+    <t>$$ASI = \sqrt{\left [ PC_{1}^{2} \times \theta_{1}^{2} \right ]+\left [ PC_{2}^{2} \times \theta_{2}^{2} \right ]}$$</t>
+  </si>
+  <si>
+    <t>[@jambhulkar_ammi_2014; @jambhulkar_genotype_2015; @jambhulkar_stability_2017]</t>
+  </si>
+  <si>
+    <t>Absolute value of the relative contribution IPCs to the interaction  $Za$</t>
+  </si>
+  <si>
+    <t>$$EV = \sum_{n=1}^{N'}\frac{\gamma_{in}^2}{N'}$$</t>
+  </si>
+  <si>
+    <t>Averages of the squared eigenvector values $EV$</t>
+  </si>
+  <si>
+    <t>Sum across environments of GEI modelled by AMMI $AMGE$</t>
+  </si>
+  <si>
+    <t>$AV_{(AMGE)}$</t>
+  </si>
+  <si>
+    <t>$W_{(AMMI)}$</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -109,13 +236,32 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -160,7 +306,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -171,13 +317,26 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -483,10 +642,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -513,61 +672,190 @@
     </row>
     <row r="2" spans="1:4" ht="150">
       <c r="A2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="1"/>
+      <c r="C2" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:4" ht="45">
       <c r="A3" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="6" t="s">
+    </row>
+    <row r="4" spans="1:4" ht="45">
+      <c r="A4" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="60">
+      <c r="A5" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C5" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="30">
+      <c r="A6" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="60">
+      <c r="A7" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="60">
+      <c r="A8" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="30">
-      <c r="A4" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="30">
-      <c r="A5" s="5" t="s">
+    </row>
+    <row r="9" spans="1:4" ht="75">
+      <c r="A9" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="30">
+      <c r="A10" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="5" t="s">
+      <c r="B10" s="2" t="s">
         <v>20</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="60">
+      <c r="A11" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="45">
+      <c r="A12" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="105">
+      <c r="A13" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="90">
+      <c r="A14" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="90">
+      <c r="A15" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="45">
+      <c r="A16" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -581,19 +869,19 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="9" t="s">
-        <v>16</v>
+      <c r="A2" s="7" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reorder  + added info
</commit_message>
<xml_diff>
--- a/vignettes/stability.xlsx
+++ b/vignettes/stability.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -29,9 +29,6 @@
     <t>AMMI stability parameter</t>
   </si>
   <si>
-    <t>xxxx</t>
-  </si>
-  <si>
     <t>[@sneller_repeatability_1997]</t>
   </si>
   <si>
@@ -56,12 +53,6 @@
     <t>Sneller</t>
   </si>
   <si>
-    <t>AMMI stability value (ASV)</t>
-  </si>
-  <si>
-    <t>Modified AMMI stability value (ASV)</t>
-  </si>
-  <si>
     <t>[@zali_evaluation_2012]</t>
   </si>
   <si>
@@ -69,9 +60,6 @@
   </si>
   <si>
     <t>[@zhang_analysis_1998]</t>
-  </si>
-  <si>
-    <t>agricolae::index.AMMI</t>
   </si>
   <si>
     <t>MASV.AMMI</t>
@@ -185,9 +173,6 @@
     <t>AVAMGE.AMMI</t>
   </si>
   <si>
-    <t>ASI.AMMI</t>
-  </si>
-  <si>
     <t>ZA.AMMI</t>
   </si>
   <si>
@@ -249,12 +234,27 @@
   <si>
     <t>$$MASI = \sqrt{ \sum_{n=1}^{N'} PC_{n}^{2} \times \theta_{n}^{2}}$$</t>
   </si>
+  <si>
+    <t>0xxxx</t>
+  </si>
+  <si>
+    <t>Modified AMMI stability value ($MASV$)</t>
+  </si>
+  <si>
+    <t>AMMI stability value ($ASV$) *</t>
+  </si>
+  <si>
+    <t>ASI.AMMI` and `MASI.AMMI</t>
+  </si>
+  <si>
+    <t>agricolae::index.AMMI` and `MASV.AMMI</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -420,7 +420,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -452,9 +452,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -486,6 +487,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -661,14 +663,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.7109375" style="3" customWidth="1"/>
     <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1"/>
@@ -676,7 +678,7 @@
     <col min="4" max="4" width="31.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30">
+    <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>3</v>
       </c>
@@ -690,238 +692,238 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="150">
+    <row r="2" spans="1:4" ht="150" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D15" s="4"/>
+    </row>
+    <row r="16" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C17" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="1:4" ht="45">
-      <c r="A3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="45">
-      <c r="A4" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="60">
-      <c r="A5" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="30">
-      <c r="A6" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="60">
-      <c r="A7" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="75">
-      <c r="A8" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C8" s="8" t="s">
+    </row>
+    <row r="18" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="C18" s="8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="75">
-      <c r="A9" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="30">
-      <c r="A10" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="60">
-      <c r="A11" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="45">
-      <c r="A12" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="105">
-      <c r="A13" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="90">
-      <c r="A14" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="90">
-      <c r="A15" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="45">
-      <c r="A16" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="30">
-      <c r="A17" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="D17" s="4"/>
-    </row>
-    <row r="18" spans="1:4" ht="30">
-      <c r="A18" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>56</v>
-      </c>
       <c r="D18" s="1" t="s">
-        <v>57</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -931,23 +933,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
After v0.1.0 pre submission tests
</commit_message>
<xml_diff>
--- a/vignettes/stability.xlsx
+++ b/vignettes/stability.xlsx
@@ -244,10 +244,10 @@
     <t>AMMI stability value ($ASV$) *</t>
   </si>
   <si>
+    <t>agricolae::index.AMMI` and `MASV.AMMI</t>
+  </si>
+  <si>
     <t>ASI.AMMI` and `MASI.AMMI</t>
-  </si>
-  <si>
-    <t>agricolae::index.AMMI` and `MASV.AMMI</t>
   </si>
 </sst>
 </file>
@@ -666,8 +666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -723,7 +723,7 @@
         <v>28</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>29</v>
@@ -751,7 +751,7 @@
         <v>61</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>18</v>

</xml_diff>